<commit_message>
Optimize plant with constant demand
</commit_message>
<xml_diff>
--- a/Data/weather_parameters.xlsx
+++ b/Data/weather_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/mans3904_ox_ac_uk/Documents/DPhil/GEOH2/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mans3904/Documents/GitHub/GEOH2-private/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{132F6D6E-AC25-4669-9B8F-787E9FC9C00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{995E0E05-B3CA-420B-835D-0F3901C96E13}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEC8A0E-CC84-1D4C-B721-D31B97F5521F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="12405" xr2:uid="{0670FC10-9C26-4E6B-94E8-052A5F11C83C}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="12400" xr2:uid="{0670FC10-9C26-4E6B-94E8-052A5F11C83C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,20 +59,27 @@
     <t>Minimum latitude (deg)</t>
   </si>
   <si>
+    <t>Maximum latitude (deg)</t>
+  </si>
+  <si>
     <t>Kenya-2022-07</t>
-  </si>
-  <si>
-    <t>Maximum latitude (deg)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,9 +105,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,29 +426,29 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>44743</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -448,7 +456,7 @@
         <v>44774</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -456,36 +464,36 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>